<commit_message>
Updated the Test Closure document
</commit_message>
<xml_diff>
--- a/VWO_Project/Defect_sheet.xlsx
+++ b/VWO_Project/Defect_sheet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Documents\Manual_Testing_Projects\vwo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Documents\Manual_Testing_Projects\VWO_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8F6BAF1-9A4C-41DE-8E6E-350CA3161153}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4371380-CA0B-40A2-9583-D7EE0FE216B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{DFFCAD63-C50D-43B0-85EC-B32DD91D370D}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="88">
   <si>
     <t>Project Name</t>
   </si>
@@ -155,13 +155,168 @@
   </si>
   <si>
     <t>Comments</t>
+  </si>
+  <si>
+    <t>DEF_001</t>
+  </si>
+  <si>
+    <t>Placeholder not visible in Email and Password fields</t>
+  </si>
+  <si>
+    <t>Sign In</t>
+  </si>
+  <si>
+    <t>1. the application URL in the browser.
+2.Check the Email and Password fields.</t>
+  </si>
+  <si>
+    <t>Placeholder text should be visible in both Email and Password fields.</t>
+  </si>
+  <si>
+    <t>Placeholder text is not visible in Email and Password fields.</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>Major</t>
+  </si>
+  <si>
+    <t>Open</t>
+  </si>
+  <si>
+    <t>Improper Error Messages Displayed for Invalid Login Credentials</t>
+  </si>
+  <si>
+    <t>For all invalid credential combinations, the system displays the same generic error message: "Invalid Credential".</t>
+  </si>
+  <si>
+    <t>Each type of invalid credential should display a specific and relevant error message, e.g.:
+Valid email + invalid password → "Incorrect password"
+Invalid email + valid password → "Email not found"</t>
+  </si>
+  <si>
+    <t>1. Enter the URL
+2.Log in with invalid admin credentials (various combinations such as valid email + invalid password, invalid email + valid password, both invalid).
+3.Observe the error message displayed for each invalid login attempt.</t>
+  </si>
+  <si>
+    <t>Error message not displayed for invalid email format</t>
+  </si>
+  <si>
+    <t>1.Enter the application URL in the browser.
+2.In the Email field, enter an invalid email format (e.g., abc@, abc.com, abc@com).
+3.Enter a valid value in the Password field.
+4.Click on the Login button.</t>
+  </si>
+  <si>
+    <t>Application should display a proper error message (e.g., “Please enter a valid email address”).</t>
+  </si>
+  <si>
+    <t>Proper error message is not displayed for invalid email format.</t>
+  </si>
+  <si>
+    <t>Sign In
+Sign In using SSO
+Forgot Password
+Start A Free Trial</t>
+  </si>
+  <si>
+    <t>P2</t>
+  </si>
+  <si>
+    <t>1.Enter the application URL in the browser.
+2.Navigate to the Login page.
+3.Observe the fields available for login.</t>
+  </si>
+  <si>
+    <t>CAPTCHA field not displayed on Sign In Page</t>
+  </si>
+  <si>
+    <t>P3</t>
+  </si>
+  <si>
+    <t>CAPTCHA field should be displayed (for security, to prevent bot logins).</t>
+  </si>
+  <si>
+    <t>CAPTCHA field is not displayed on the Sign In page.</t>
+  </si>
+  <si>
+    <t>DEF_002</t>
+  </si>
+  <si>
+    <t>DEF_003</t>
+  </si>
+  <si>
+    <t>DEF_004</t>
+  </si>
+  <si>
+    <t>Dark and Light theme option not available</t>
+  </si>
+  <si>
+    <t>1.Open the application URL in the browser.
+2.Check the UI options for theme (Dark mode / Light mode).</t>
+  </si>
+  <si>
+    <t>User should be able to switch between Dark and Light themes (for accessibility &amp; better user experience).</t>
+  </si>
+  <si>
+    <t>Dark and Light theme option is not available.</t>
+  </si>
+  <si>
+    <t>Leading/Trailing spaces in Email field not trimmed</t>
+  </si>
+  <si>
+    <t>Critical</t>
+  </si>
+  <si>
+    <t>1.Open the application URL in the browser.
+2.In the Email field, enter a valid email address with spaces (e.g., " testuser@email.com ").
+3.Enter a valid password.
+4.Click the Sign in button.</t>
+  </si>
+  <si>
+    <t>Application should trim the leading and trailing spaces and allow login with the valid email.</t>
+  </si>
+  <si>
+    <t>Spaces are not trimmed → login fails / invalid email error shown.</t>
+  </si>
+  <si>
+    <t>No validation popup displayed when Email field is left blank</t>
+  </si>
+  <si>
+    <t>1.Open the application URL in the browser.
+2.Leave the Email field blank.
+3.Enter a valid password.
+4.Click the Sign in button.</t>
+  </si>
+  <si>
+    <t>Application should display a validation popup/message (e.g., “Please enter your email address”).</t>
+  </si>
+  <si>
+    <t>No validation popup/message is displayed when Email field is left blank.</t>
+  </si>
+  <si>
+    <t>DEF_005</t>
+  </si>
+  <si>
+    <t>DEF_006</t>
+  </si>
+  <si>
+    <t>DEF_007</t>
+  </si>
+  <si>
+    <t>Assign to Dev</t>
+  </si>
+  <si>
+    <t>demo website</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -200,6 +355,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -209,7 +370,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -333,56 +494,83 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -712,185 +900,185 @@
   <sheetData>
     <row r="2" spans="6:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="6:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="2"/>
+      <c r="G3" s="15"/>
     </row>
     <row r="4" spans="6:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="6:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="6:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F6" s="7" t="s">
+      <c r="F6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G6" s="8">
+      <c r="G6" s="6">
         <v>45146</v>
       </c>
     </row>
     <row r="10" spans="6:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="6:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F11" s="14" t="s">
+      <c r="F11" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="G11" s="15" t="s">
+      <c r="G11" s="13" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="12" spans="6:7" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="F12" s="12" t="s">
+      <c r="F12" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="G12" s="13" t="s">
+      <c r="G12" s="11" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="13" spans="6:7" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="F13" s="9" t="s">
+      <c r="F13" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G13" s="10" t="s">
+      <c r="G13" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="14" spans="6:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="F14" s="9" t="s">
+      <c r="F14" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G14" s="10" t="s">
+      <c r="G14" s="8" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="15" spans="6:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="F15" s="9" t="s">
+      <c r="F15" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G15" s="10" t="s">
+      <c r="G15" s="8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="6:7" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="F16" s="9" t="s">
+    <row r="16" spans="6:7" ht="63" x14ac:dyDescent="0.25">
+      <c r="F16" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="G16" s="10" t="s">
+      <c r="G16" s="8" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="17" spans="6:7" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="F17" s="9" t="s">
+      <c r="F17" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="G17" s="10" t="s">
+      <c r="G17" s="8" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="18" spans="6:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="F18" s="9" t="s">
+      <c r="F18" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="G18" s="10" t="s">
+      <c r="G18" s="8" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="19" spans="6:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="F19" s="9" t="s">
+      <c r="F19" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G19" s="10" t="s">
+      <c r="G19" s="8" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="20" spans="6:7" ht="63" x14ac:dyDescent="0.25">
-      <c r="F20" s="9" t="s">
+      <c r="F20" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G20" s="10" t="s">
+      <c r="G20" s="8" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="21" spans="6:7" ht="63" x14ac:dyDescent="0.25">
-      <c r="F21" s="9" t="s">
+      <c r="F21" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="G21" s="10" t="s">
+      <c r="G21" s="8" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="6:7" ht="63" x14ac:dyDescent="0.25">
-      <c r="F22" s="9" t="s">
+    <row r="22" spans="6:7" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="F22" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="G22" s="10" t="s">
+      <c r="G22" s="8" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="23" spans="6:7" ht="63" x14ac:dyDescent="0.25">
-      <c r="F23" s="9" t="s">
+      <c r="F23" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="G23" s="10" t="s">
+      <c r="G23" s="8" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="24" spans="6:7" ht="63" x14ac:dyDescent="0.25">
-      <c r="F24" s="9" t="s">
+    <row r="24" spans="6:7" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="F24" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="G24" s="10" t="s">
+      <c r="G24" s="8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="25" spans="6:7" ht="63" x14ac:dyDescent="0.25">
-      <c r="F25" s="9" t="s">
+      <c r="F25" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="G25" s="10" t="s">
+      <c r="G25" s="8" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="26" spans="6:7" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="F26" s="9" t="s">
+      <c r="F26" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="G26" s="10" t="s">
+      <c r="G26" s="8" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="27" spans="6:7" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="F27" s="9" t="s">
+      <c r="F27" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="G27" s="10" t="s">
+      <c r="G27" s="8" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="28" spans="6:7" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="F28" s="9" t="s">
+      <c r="F28" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="G28" s="10" t="s">
+      <c r="G28" s="8" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="29" spans="6:7" ht="48" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F29" s="11" t="s">
+      <c r="F29" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="G29" s="10" t="s">
+      <c r="G29" s="8" t="s">
         <v>41</v>
       </c>
     </row>
@@ -904,88 +1092,412 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3561D3B7-399B-4A11-8964-E804366C30EC}">
-  <dimension ref="A1:R1"/>
+  <dimension ref="A1:R8"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+    <sheetView topLeftCell="H4" workbookViewId="0">
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" customWidth="1"/>
-    <col min="6" max="6" width="19.42578125" customWidth="1"/>
-    <col min="7" max="7" width="17.42578125" customWidth="1"/>
-    <col min="8" max="8" width="16" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" customWidth="1"/>
+    <col min="6" max="6" width="33.28515625" customWidth="1"/>
+    <col min="7" max="7" width="23.28515625" customWidth="1"/>
+    <col min="8" max="8" width="22.28515625" customWidth="1"/>
     <col min="9" max="9" width="15.7109375" customWidth="1"/>
     <col min="10" max="10" width="13.5703125" customWidth="1"/>
     <col min="11" max="11" width="14" customWidth="1"/>
-    <col min="12" max="12" width="12.85546875" customWidth="1"/>
+    <col min="12" max="12" width="14.140625" customWidth="1"/>
     <col min="13" max="13" width="13.85546875" customWidth="1"/>
-    <col min="14" max="14" width="12.140625" customWidth="1"/>
+    <col min="14" max="14" width="14" customWidth="1"/>
     <col min="15" max="15" width="12.85546875" customWidth="1"/>
     <col min="16" max="16" width="13.85546875" customWidth="1"/>
     <col min="17" max="17" width="14.28515625" customWidth="1"/>
     <col min="18" max="18" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:18" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="K1" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="L1" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="M1" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="N1" s="9" t="s">
+      <c r="N1" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="O1" s="9" t="s">
+      <c r="O1" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="P1" s="9" t="s">
+      <c r="P1" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="Q1" s="9" t="s">
+      <c r="Q1" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="R1" s="11" t="s">
+      <c r="R1" s="17" t="s">
         <v>42</v>
       </c>
     </row>
+    <row r="2" spans="1:18" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="G2" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="H2" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="K2" s="19">
+        <v>45146</v>
+      </c>
+      <c r="L2" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="M2" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="N2" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="O2" s="16"/>
+      <c r="P2" s="16"/>
+      <c r="Q2" s="16"/>
+      <c r="R2" s="16"/>
+    </row>
+    <row r="3" spans="1:18" ht="151.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="F3" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="H3" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="K3" s="19">
+        <v>45146</v>
+      </c>
+      <c r="L3" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="M3" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="N3" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="O3" s="16"/>
+      <c r="P3" s="16"/>
+      <c r="Q3" s="16"/>
+      <c r="R3" s="16"/>
+    </row>
+    <row r="4" spans="1:18" ht="120" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="F4" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="G4" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="H4" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="K4" s="19">
+        <v>45146</v>
+      </c>
+      <c r="L4" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="M4" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="N4" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="O4" s="16"/>
+      <c r="P4" s="16"/>
+      <c r="Q4" s="16"/>
+      <c r="R4" s="16"/>
+    </row>
+    <row r="5" spans="1:18" ht="75" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="F5" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="G5" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="H5" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="I5" s="16"/>
+      <c r="J5" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="K5" s="19">
+        <v>45146</v>
+      </c>
+      <c r="L5" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="M5" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="N5" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="O5" s="16"/>
+      <c r="P5" s="16"/>
+      <c r="Q5" s="16"/>
+      <c r="R5" s="16"/>
+    </row>
+    <row r="6" spans="1:18" ht="75" x14ac:dyDescent="0.25">
+      <c r="A6" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="E6" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="F6" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="G6" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="H6" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="K6" s="19">
+        <v>45147</v>
+      </c>
+      <c r="L6" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="M6" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="N6" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="O6" s="16"/>
+      <c r="P6" s="16"/>
+      <c r="Q6" s="16"/>
+      <c r="R6" s="16"/>
+    </row>
+    <row r="7" spans="1:18" ht="105" x14ac:dyDescent="0.25">
+      <c r="A7" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="F7" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="G7" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="H7" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="I7" s="16"/>
+      <c r="J7" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="K7" s="19">
+        <v>45147</v>
+      </c>
+      <c r="L7" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="M7" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="N7" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="O7" s="16"/>
+      <c r="P7" s="16"/>
+      <c r="Q7" s="16"/>
+      <c r="R7" s="16"/>
+    </row>
+    <row r="8" spans="1:18" ht="75" x14ac:dyDescent="0.25">
+      <c r="A8" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="F8" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="H8" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="I8" s="16"/>
+      <c r="J8" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="K8" s="19">
+        <v>45147</v>
+      </c>
+      <c r="L8" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="M8" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="N8" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="O8" s="16"/>
+      <c r="P8" s="16"/>
+      <c r="Q8" s="16"/>
+      <c r="R8" s="16"/>
+    </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>